<commit_message>
small change in load state of ins_cache
</commit_message>
<xml_diff>
--- a/referenceAnswer.xlsx
+++ b/referenceAnswer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FPGA\AP_5v_1clk\AP_5v.srcs\sources_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FPGA\AP_5v_1clk\AP_5v.srcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ACD2C90-4C4E-4281-A72E-D00562B80B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6983E2FD-6A77-408A-B6EC-2B4CAAA91969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4330" yWindow="4520" windowWidth="28800" windowHeight="15460" xr2:uid="{56AC80A6-65A3-4EDC-A59A-A248A5A2B952}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{56AC80A6-65A3-4EDC-A59A-A248A5A2B952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C723547-35F5-4F73-B7B9-277B659E342A}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -952,22 +952,22 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -982,22 +982,22 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I19">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1012,22 +1012,22 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I20">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1042,22 +1042,22 @@
         <v>20</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1072,22 +1072,22 @@
         <v>21</v>
       </c>
       <c r="D22">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E22">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F22">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H22">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I22">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1102,22 +1102,22 @@
         <v>22</v>
       </c>
       <c r="D23">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E23">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F23">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G23">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H23">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I23">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1132,22 +1132,22 @@
         <v>23</v>
       </c>
       <c r="D24">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E24">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F24">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G24">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H24">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I24">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1162,22 +1162,22 @@
         <v>24</v>
       </c>
       <c r="D25">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E25">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F25">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G25">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H25">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I25">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1192,22 +1192,22 @@
         <v>25</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F26">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G26">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H26">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I26">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1222,22 +1222,22 @@
         <v>26</v>
       </c>
       <c r="D27">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E27">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F27">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G27">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H27">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I27">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1252,22 +1252,22 @@
         <v>27</v>
       </c>
       <c r="D28">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E28">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F28">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G28">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H28">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="I28">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1282,22 +1282,22 @@
         <v>28</v>
       </c>
       <c r="D29">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F29">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G29">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H29">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I29">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1312,22 +1312,22 @@
         <v>29</v>
       </c>
       <c r="D30">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E30">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F30">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G30">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="H30">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="I30">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1342,22 +1342,22 @@
         <v>30</v>
       </c>
       <c r="D31">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E31">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F31">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G31">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H31">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I31">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1372,22 +1372,22 @@
         <v>31</v>
       </c>
       <c r="D32">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E32">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F32">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G32">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="H32">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="I32">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1402,22 +1402,22 @@
         <v>32</v>
       </c>
       <c r="D33">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E33">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F33">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G33">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H33">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I33">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:9">

</xml_diff>

<commit_message>
add the auto check function in testbench and controller
</commit_message>
<xml_diff>
--- a/referenceAnswer.xlsx
+++ b/referenceAnswer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FPGA\AP_5v_1clk\AP_5v.srcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6983E2FD-6A77-408A-B6EC-2B4CAAA91969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDB4C63-64C5-4997-BBF6-6F28120A5FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{56AC80A6-65A3-4EDC-A59A-A248A5A2B952}"/>
   </bookViews>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C723547-35F5-4F73-B7B9-277B659E342A}">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -431,7 +431,7 @@
     <col min="1" max="1" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>4096</v>
       </c>
@@ -489,8 +489,12 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="str">
+        <f>DEC2BIN(I2,8)</f>
+        <v>00000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>4097</v>
       </c>
@@ -519,8 +523,12 @@
       <c r="I3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="1">DEC2BIN(I3,8)</f>
+        <v>00000010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>4098</v>
       </c>
@@ -549,8 +557,12 @@
       <c r="I4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v>00000011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>4099</v>
       </c>
@@ -579,8 +591,12 @@
       <c r="I5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>00000100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4100</v>
       </c>
@@ -609,8 +625,12 @@
       <c r="I6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>00000101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>4101</v>
       </c>
@@ -639,8 +659,12 @@
       <c r="I7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>00000110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>4102</v>
       </c>
@@ -669,8 +693,12 @@
       <c r="I8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>00000111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>4103</v>
       </c>
@@ -699,8 +727,12 @@
       <c r="I9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>00001000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>4104</v>
       </c>
@@ -729,8 +761,12 @@
       <c r="I10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v>00001001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>4105</v>
       </c>
@@ -759,8 +795,12 @@
       <c r="I11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v>00001010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>4106</v>
       </c>
@@ -789,8 +829,12 @@
       <c r="I12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v>00001011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>4107</v>
       </c>
@@ -819,8 +863,12 @@
       <c r="I13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v>00001100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>4108</v>
       </c>
@@ -849,8 +897,12 @@
       <c r="I14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>00001101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>4109</v>
       </c>
@@ -879,8 +931,12 @@
       <c r="I15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>00001110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>4110</v>
       </c>
@@ -909,8 +965,12 @@
       <c r="I16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>00001111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>4111</v>
       </c>
@@ -939,8 +999,12 @@
       <c r="I17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>4112</v>
       </c>
@@ -969,8 +1033,12 @@
       <c r="I18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>4113</v>
       </c>
@@ -999,8 +1067,12 @@
       <c r="I19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>4114</v>
       </c>
@@ -1029,8 +1101,12 @@
       <c r="I20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>4115</v>
       </c>
@@ -1059,8 +1135,12 @@
       <c r="I21">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>4116</v>
       </c>
@@ -1089,8 +1169,12 @@
       <c r="I22">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>4117</v>
       </c>
@@ -1119,8 +1203,12 @@
       <c r="I23">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>4118</v>
       </c>
@@ -1149,8 +1237,12 @@
       <c r="I24">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>4119</v>
       </c>
@@ -1179,8 +1271,12 @@
       <c r="I25">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>4120</v>
       </c>
@@ -1209,8 +1305,12 @@
       <c r="I26">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>4121</v>
       </c>
@@ -1239,8 +1339,12 @@
       <c r="I27">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>4122</v>
       </c>
@@ -1269,8 +1373,12 @@
       <c r="I28">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>4123</v>
       </c>
@@ -1299,8 +1407,12 @@
       <c r="I29">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>4124</v>
       </c>
@@ -1329,8 +1441,12 @@
       <c r="I30">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>4125</v>
       </c>
@@ -1359,8 +1475,12 @@
       <c r="I31">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>4126</v>
       </c>
@@ -1389,8 +1509,12 @@
       <c r="I32">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>4127</v>
       </c>
@@ -1419,8 +1543,12 @@
       <c r="I33">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" t="str">
+        <f t="shared" si="1"/>
+        <v>00010000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>4128</v>
       </c>
@@ -1449,8 +1577,12 @@
       <c r="I34">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" t="str">
+        <f t="shared" si="1"/>
+        <v>00010010</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>4129</v>
       </c>
@@ -1479,8 +1611,12 @@
       <c r="I35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" t="str">
+        <f t="shared" si="1"/>
+        <v>00010100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>4130</v>
       </c>
@@ -1509,8 +1645,12 @@
       <c r="I36">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" t="str">
+        <f t="shared" si="1"/>
+        <v>00010110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>4131</v>
       </c>
@@ -1539,8 +1679,12 @@
       <c r="I37">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" t="str">
+        <f t="shared" si="1"/>
+        <v>00011000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>4132</v>
       </c>
@@ -1569,8 +1713,12 @@
       <c r="I38">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" t="str">
+        <f t="shared" si="1"/>
+        <v>00011010</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>4133</v>
       </c>
@@ -1599,8 +1747,12 @@
       <c r="I39">
         <v>28</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" t="str">
+        <f t="shared" si="1"/>
+        <v>00011100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>4134</v>
       </c>
@@ -1629,8 +1781,12 @@
       <c r="I40">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" t="str">
+        <f t="shared" si="1"/>
+        <v>00011110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>4135</v>
       </c>
@@ -1659,8 +1815,12 @@
       <c r="I41">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" t="str">
+        <f t="shared" si="1"/>
+        <v>00100000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>4136</v>
       </c>
@@ -1689,8 +1849,12 @@
       <c r="I42">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" t="str">
+        <f t="shared" si="1"/>
+        <v>00100010</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>4137</v>
       </c>
@@ -1719,8 +1883,12 @@
       <c r="I43">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" t="str">
+        <f t="shared" si="1"/>
+        <v>00100100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>4138</v>
       </c>
@@ -1749,8 +1917,12 @@
       <c r="I44">
         <v>38</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" t="str">
+        <f t="shared" si="1"/>
+        <v>00100110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>4139</v>
       </c>
@@ -1779,8 +1951,12 @@
       <c r="I45">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" t="str">
+        <f t="shared" si="1"/>
+        <v>00101000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>4140</v>
       </c>
@@ -1809,8 +1985,12 @@
       <c r="I46">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" t="str">
+        <f t="shared" si="1"/>
+        <v>00101010</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>4141</v>
       </c>
@@ -1839,8 +2019,12 @@
       <c r="I47">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" t="str">
+        <f t="shared" si="1"/>
+        <v>00101100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>4142</v>
       </c>
@@ -1869,8 +2053,12 @@
       <c r="I48">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" t="str">
+        <f t="shared" si="1"/>
+        <v>00101110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>4143</v>
       </c>
@@ -1899,8 +2087,12 @@
       <c r="I49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" t="str">
+        <f t="shared" si="1"/>
+        <v>00110000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>4144</v>
       </c>
@@ -1929,8 +2121,12 @@
       <c r="I50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" t="str">
+        <f t="shared" si="1"/>
+        <v>00110001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>4145</v>
       </c>
@@ -1959,8 +2155,12 @@
       <c r="I51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" t="str">
+        <f t="shared" si="1"/>
+        <v>00110010</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>4146</v>
       </c>
@@ -1989,8 +2189,12 @@
       <c r="I52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" t="str">
+        <f t="shared" si="1"/>
+        <v>00110011</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>4147</v>
       </c>
@@ -2019,8 +2223,12 @@
       <c r="I53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" t="str">
+        <f t="shared" si="1"/>
+        <v>00110100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>4148</v>
       </c>
@@ -2049,8 +2257,12 @@
       <c r="I54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" t="str">
+        <f t="shared" si="1"/>
+        <v>00110101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>4149</v>
       </c>
@@ -2079,8 +2291,12 @@
       <c r="I55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" t="str">
+        <f t="shared" si="1"/>
+        <v>00110110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>4150</v>
       </c>
@@ -2109,8 +2325,12 @@
       <c r="I56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" t="str">
+        <f t="shared" si="1"/>
+        <v>00110111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>4151</v>
       </c>
@@ -2139,8 +2359,12 @@
       <c r="I57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" t="str">
+        <f t="shared" si="1"/>
+        <v>00111000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>4152</v>
       </c>
@@ -2169,8 +2393,12 @@
       <c r="I58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" t="str">
+        <f t="shared" si="1"/>
+        <v>00111001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>4153</v>
       </c>
@@ -2199,8 +2427,12 @@
       <c r="I59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" t="str">
+        <f t="shared" si="1"/>
+        <v>00111010</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>4154</v>
       </c>
@@ -2229,8 +2461,12 @@
       <c r="I60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" t="str">
+        <f t="shared" si="1"/>
+        <v>00111011</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>4155</v>
       </c>
@@ -2259,8 +2495,12 @@
       <c r="I61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" t="str">
+        <f t="shared" si="1"/>
+        <v>00111100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>4156</v>
       </c>
@@ -2289,8 +2529,12 @@
       <c r="I62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" t="str">
+        <f t="shared" si="1"/>
+        <v>00111101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>4157</v>
       </c>
@@ -2319,8 +2563,12 @@
       <c r="I63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" t="str">
+        <f t="shared" si="1"/>
+        <v>00111110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>4158</v>
       </c>
@@ -2349,8 +2597,12 @@
       <c r="I64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" t="str">
+        <f t="shared" si="1"/>
+        <v>00111111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>4159</v>
       </c>
@@ -2379,8 +2631,12 @@
       <c r="I65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" t="str">
+        <f t="shared" si="1"/>
+        <v>01000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>4160</v>
       </c>
@@ -2409,13 +2665,17 @@
       <c r="I66">
         <v>-122</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" t="str">
+        <f>DEC2BIN(I66,8)</f>
+        <v>1110000110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>4161</v>
       </c>
       <c r="B67" s="1" t="str">
-        <f t="shared" ref="B67:B129" si="1">DEC2HEX(A67,4)</f>
+        <f t="shared" ref="B67:B129" si="2">DEC2HEX(A67,4)</f>
         <v>1041</v>
       </c>
       <c r="C67">
@@ -2439,13 +2699,17 @@
       <c r="I67">
         <v>-116</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J129" si="3">DEC2BIN(I67,8)</f>
+        <v>1110001100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>4162</v>
       </c>
       <c r="B68" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1042</v>
       </c>
       <c r="C68">
@@ -2469,13 +2733,17 @@
       <c r="I68">
         <v>-110</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68" t="str">
+        <f t="shared" si="3"/>
+        <v>1110010010</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>4163</v>
       </c>
       <c r="B69" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1043</v>
       </c>
       <c r="C69">
@@ -2499,13 +2767,17 @@
       <c r="I69">
         <v>-104</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69" t="str">
+        <f t="shared" si="3"/>
+        <v>1110011000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>4164</v>
       </c>
       <c r="B70" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1044</v>
       </c>
       <c r="C70">
@@ -2529,13 +2801,17 @@
       <c r="I70">
         <v>-98</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70" t="str">
+        <f t="shared" si="3"/>
+        <v>1110011110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>4165</v>
       </c>
       <c r="B71" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1045</v>
       </c>
       <c r="C71">
@@ -2559,13 +2835,17 @@
       <c r="I71">
         <v>-92</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71" t="str">
+        <f t="shared" si="3"/>
+        <v>1110100100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>4166</v>
       </c>
       <c r="B72" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1046</v>
       </c>
       <c r="C72">
@@ -2589,13 +2869,17 @@
       <c r="I72">
         <v>-86</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72" t="str">
+        <f t="shared" si="3"/>
+        <v>1110101010</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>4167</v>
       </c>
       <c r="B73" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1047</v>
       </c>
       <c r="C73">
@@ -2619,13 +2903,17 @@
       <c r="I73">
         <v>-80</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73" t="str">
+        <f t="shared" si="3"/>
+        <v>1110110000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>4168</v>
       </c>
       <c r="B74" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1048</v>
       </c>
       <c r="C74">
@@ -2649,13 +2937,17 @@
       <c r="I74">
         <v>-74</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74" t="str">
+        <f t="shared" si="3"/>
+        <v>1110110110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>4169</v>
       </c>
       <c r="B75" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1049</v>
       </c>
       <c r="C75">
@@ -2679,13 +2971,17 @@
       <c r="I75">
         <v>-68</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75" t="str">
+        <f t="shared" si="3"/>
+        <v>1110111100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>4170</v>
       </c>
       <c r="B76" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104A</v>
       </c>
       <c r="C76">
@@ -2709,13 +3005,17 @@
       <c r="I76">
         <v>-62</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76" t="str">
+        <f t="shared" si="3"/>
+        <v>1111000010</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>4171</v>
       </c>
       <c r="B77" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104B</v>
       </c>
       <c r="C77">
@@ -2739,13 +3039,17 @@
       <c r="I77">
         <v>-56</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77" t="str">
+        <f t="shared" si="3"/>
+        <v>1111001000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>4172</v>
       </c>
       <c r="B78" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104C</v>
       </c>
       <c r="C78">
@@ -2769,13 +3073,17 @@
       <c r="I78">
         <v>-50</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" t="str">
+        <f t="shared" si="3"/>
+        <v>1111001110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>4173</v>
       </c>
       <c r="B79" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104D</v>
       </c>
       <c r="C79">
@@ -2799,13 +3107,17 @@
       <c r="I79">
         <v>-44</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79" t="str">
+        <f t="shared" si="3"/>
+        <v>1111010100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>4174</v>
       </c>
       <c r="B80" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104E</v>
       </c>
       <c r="C80">
@@ -2829,13 +3141,17 @@
       <c r="I80">
         <v>-38</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" t="str">
+        <f t="shared" si="3"/>
+        <v>1111011010</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>4175</v>
       </c>
       <c r="B81" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104F</v>
       </c>
       <c r="C81">
@@ -2859,13 +3175,17 @@
       <c r="I81">
         <v>-32</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" t="str">
+        <f t="shared" si="3"/>
+        <v>1111100000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>4176</v>
       </c>
       <c r="B82" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1050</v>
       </c>
       <c r="C82">
@@ -2889,13 +3209,17 @@
       <c r="I82">
         <v>116</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" t="str">
+        <f t="shared" si="3"/>
+        <v>01110100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>4177</v>
       </c>
       <c r="B83" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1051</v>
       </c>
       <c r="C83">
@@ -2919,13 +3243,17 @@
       <c r="I83">
         <v>120</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" t="str">
+        <f t="shared" si="3"/>
+        <v>01111000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>4178</v>
       </c>
       <c r="B84" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1052</v>
       </c>
       <c r="C84">
@@ -2949,13 +3277,17 @@
       <c r="I84">
         <v>124</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" t="str">
+        <f t="shared" si="3"/>
+        <v>01111100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>4179</v>
       </c>
       <c r="B85" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1053</v>
       </c>
       <c r="C85">
@@ -2979,13 +3311,17 @@
       <c r="I85">
         <v>-128</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" t="str">
+        <f t="shared" si="3"/>
+        <v>1110000000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>4180</v>
       </c>
       <c r="B86" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1054</v>
       </c>
       <c r="C86">
@@ -3009,13 +3345,17 @@
       <c r="I86">
         <v>-124</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" t="str">
+        <f t="shared" si="3"/>
+        <v>1110000100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>4181</v>
       </c>
       <c r="B87" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1055</v>
       </c>
       <c r="C87">
@@ -3039,13 +3379,17 @@
       <c r="I87">
         <v>-120</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" t="str">
+        <f t="shared" si="3"/>
+        <v>1110001000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>4182</v>
       </c>
       <c r="B88" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1056</v>
       </c>
       <c r="C88">
@@ -3069,13 +3413,17 @@
       <c r="I88">
         <v>-116</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" t="str">
+        <f t="shared" si="3"/>
+        <v>1110001100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>4183</v>
       </c>
       <c r="B89" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1057</v>
       </c>
       <c r="C89">
@@ -3099,13 +3447,17 @@
       <c r="I89">
         <v>-112</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" t="str">
+        <f t="shared" si="3"/>
+        <v>1110010000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>4184</v>
       </c>
       <c r="B90" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1058</v>
       </c>
       <c r="C90">
@@ -3129,13 +3481,17 @@
       <c r="I90">
         <v>-108</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" t="str">
+        <f t="shared" si="3"/>
+        <v>1110010100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>4185</v>
       </c>
       <c r="B91" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1059</v>
       </c>
       <c r="C91">
@@ -3159,13 +3515,17 @@
       <c r="I91">
         <v>-104</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" t="str">
+        <f t="shared" si="3"/>
+        <v>1110011000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>4186</v>
       </c>
       <c r="B92" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105A</v>
       </c>
       <c r="C92">
@@ -3189,13 +3549,17 @@
       <c r="I92">
         <v>-100</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92" t="str">
+        <f t="shared" si="3"/>
+        <v>1110011100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>4187</v>
       </c>
       <c r="B93" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105B</v>
       </c>
       <c r="C93">
@@ -3219,13 +3583,17 @@
       <c r="I93">
         <v>-96</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93" t="str">
+        <f t="shared" si="3"/>
+        <v>1110100000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>4188</v>
       </c>
       <c r="B94" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105C</v>
       </c>
       <c r="C94">
@@ -3249,13 +3617,17 @@
       <c r="I94">
         <v>-92</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94" t="str">
+        <f t="shared" si="3"/>
+        <v>1110100100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>4189</v>
       </c>
       <c r="B95" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105D</v>
       </c>
       <c r="C95">
@@ -3279,13 +3651,17 @@
       <c r="I95">
         <v>-88</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95" t="str">
+        <f t="shared" si="3"/>
+        <v>1110101000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>4190</v>
       </c>
       <c r="B96" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105E</v>
       </c>
       <c r="C96">
@@ -3309,13 +3685,17 @@
       <c r="I96">
         <v>-84</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96" t="str">
+        <f t="shared" si="3"/>
+        <v>1110101100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>4191</v>
       </c>
       <c r="B97" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105F</v>
       </c>
       <c r="C97">
@@ -3339,13 +3719,17 @@
       <c r="I97">
         <v>-80</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97" t="str">
+        <f t="shared" si="3"/>
+        <v>1110110000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>4192</v>
       </c>
       <c r="B98" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1060</v>
       </c>
       <c r="C98">
@@ -3369,13 +3753,17 @@
       <c r="I98">
         <v>-116</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98" t="str">
+        <f t="shared" si="3"/>
+        <v>1110001100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>4193</v>
       </c>
       <c r="B99" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1061</v>
       </c>
       <c r="C99">
@@ -3399,13 +3787,17 @@
       <c r="I99">
         <v>-120</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="J99" t="str">
+        <f t="shared" si="3"/>
+        <v>1110001000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>4194</v>
       </c>
       <c r="B100" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1062</v>
       </c>
       <c r="C100">
@@ -3429,13 +3821,17 @@
       <c r="I100">
         <v>-124</v>
       </c>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="J100" t="str">
+        <f t="shared" si="3"/>
+        <v>1110000100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>4195</v>
       </c>
       <c r="B101" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1063</v>
       </c>
       <c r="C101">
@@ -3459,13 +3855,17 @@
       <c r="I101">
         <v>-128</v>
       </c>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="J101" t="str">
+        <f t="shared" si="3"/>
+        <v>1110000000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>4196</v>
       </c>
       <c r="B102" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1064</v>
       </c>
       <c r="C102">
@@ -3489,13 +3889,17 @@
       <c r="I102">
         <v>124</v>
       </c>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="J102" t="str">
+        <f t="shared" si="3"/>
+        <v>01111100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>4197</v>
       </c>
       <c r="B103" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1065</v>
       </c>
       <c r="C103">
@@ -3519,13 +3923,17 @@
       <c r="I103">
         <v>120</v>
       </c>
-    </row>
-    <row r="104" spans="1:9">
+      <c r="J103" t="str">
+        <f t="shared" si="3"/>
+        <v>01111000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>4198</v>
       </c>
       <c r="B104" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1066</v>
       </c>
       <c r="C104">
@@ -3549,13 +3957,17 @@
       <c r="I104">
         <v>116</v>
       </c>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="J104" t="str">
+        <f t="shared" si="3"/>
+        <v>01110100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>4199</v>
       </c>
       <c r="B105" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1067</v>
       </c>
       <c r="C105">
@@ -3579,13 +3991,17 @@
       <c r="I105">
         <v>112</v>
       </c>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="J105" t="str">
+        <f t="shared" si="3"/>
+        <v>01110000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>4200</v>
       </c>
       <c r="B106" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1068</v>
       </c>
       <c r="C106">
@@ -3609,13 +4025,17 @@
       <c r="I106">
         <v>108</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106" t="str">
+        <f t="shared" si="3"/>
+        <v>01101100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>4201</v>
       </c>
       <c r="B107" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1069</v>
       </c>
       <c r="C107">
@@ -3639,13 +4059,17 @@
       <c r="I107">
         <v>104</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="J107" t="str">
+        <f t="shared" si="3"/>
+        <v>01101000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>4202</v>
       </c>
       <c r="B108" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106A</v>
       </c>
       <c r="C108">
@@ -3669,13 +4093,17 @@
       <c r="I108">
         <v>100</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="J108" t="str">
+        <f t="shared" si="3"/>
+        <v>01100100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>4203</v>
       </c>
       <c r="B109" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106B</v>
       </c>
       <c r="C109">
@@ -3699,13 +4127,17 @@
       <c r="I109">
         <v>96</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="J109" t="str">
+        <f t="shared" si="3"/>
+        <v>01100000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>4204</v>
       </c>
       <c r="B110" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106C</v>
       </c>
       <c r="C110">
@@ -3729,13 +4161,17 @@
       <c r="I110">
         <v>92</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="J110" t="str">
+        <f t="shared" si="3"/>
+        <v>01011100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>4205</v>
       </c>
       <c r="B111" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106D</v>
       </c>
       <c r="C111">
@@ -3759,13 +4195,17 @@
       <c r="I111">
         <v>88</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="J111" t="str">
+        <f t="shared" si="3"/>
+        <v>01011000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>4206</v>
       </c>
       <c r="B112" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106E</v>
       </c>
       <c r="C112">
@@ -3789,13 +4229,17 @@
       <c r="I112">
         <v>84</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112" t="str">
+        <f t="shared" si="3"/>
+        <v>01010100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>4207</v>
       </c>
       <c r="B113" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106F</v>
       </c>
       <c r="C113">
@@ -3819,13 +4263,17 @@
       <c r="I113">
         <v>80</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113" t="str">
+        <f t="shared" si="3"/>
+        <v>01010000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>4208</v>
       </c>
       <c r="B114" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1070</v>
       </c>
       <c r="C114">
@@ -3849,13 +4297,17 @@
       <c r="I114">
         <v>122</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" t="str">
+        <f t="shared" si="3"/>
+        <v>01111010</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>4209</v>
       </c>
       <c r="B115" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1071</v>
       </c>
       <c r="C115">
@@ -3879,13 +4331,17 @@
       <c r="I115">
         <v>116</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115" t="str">
+        <f t="shared" si="3"/>
+        <v>01110100</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>4210</v>
       </c>
       <c r="B116" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1072</v>
       </c>
       <c r="C116">
@@ -3909,13 +4365,17 @@
       <c r="I116">
         <v>110</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116" t="str">
+        <f t="shared" si="3"/>
+        <v>01101110</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>4211</v>
       </c>
       <c r="B117" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1073</v>
       </c>
       <c r="C117">
@@ -3939,13 +4399,17 @@
       <c r="I117">
         <v>104</v>
       </c>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="J117" t="str">
+        <f t="shared" si="3"/>
+        <v>01101000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>4212</v>
       </c>
       <c r="B118" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1074</v>
       </c>
       <c r="C118">
@@ -3969,13 +4433,17 @@
       <c r="I118">
         <v>98</v>
       </c>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="J118" t="str">
+        <f t="shared" si="3"/>
+        <v>01100010</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>4213</v>
       </c>
       <c r="B119" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1075</v>
       </c>
       <c r="C119">
@@ -3999,13 +4467,17 @@
       <c r="I119">
         <v>92</v>
       </c>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="J119" t="str">
+        <f t="shared" si="3"/>
+        <v>01011100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>4214</v>
       </c>
       <c r="B120" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1076</v>
       </c>
       <c r="C120">
@@ -4029,13 +4501,17 @@
       <c r="I120">
         <v>86</v>
       </c>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="J120" t="str">
+        <f t="shared" si="3"/>
+        <v>01010110</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>4215</v>
       </c>
       <c r="B121" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1077</v>
       </c>
       <c r="C121">
@@ -4059,13 +4535,17 @@
       <c r="I121">
         <v>80</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="J121" t="str">
+        <f t="shared" si="3"/>
+        <v>01010000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>4216</v>
       </c>
       <c r="B122" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1078</v>
       </c>
       <c r="C122">
@@ -4089,13 +4569,17 @@
       <c r="I122">
         <v>74</v>
       </c>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="J122" t="str">
+        <f t="shared" si="3"/>
+        <v>01001010</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>4217</v>
       </c>
       <c r="B123" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1079</v>
       </c>
       <c r="C123">
@@ -4119,13 +4603,17 @@
       <c r="I123">
         <v>68</v>
       </c>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="J123" t="str">
+        <f t="shared" si="3"/>
+        <v>01000100</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>4218</v>
       </c>
       <c r="B124" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107A</v>
       </c>
       <c r="C124">
@@ -4149,13 +4637,17 @@
       <c r="I124">
         <v>62</v>
       </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="J124" t="str">
+        <f t="shared" si="3"/>
+        <v>00111110</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>4219</v>
       </c>
       <c r="B125" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107B</v>
       </c>
       <c r="C125">
@@ -4179,13 +4671,17 @@
       <c r="I125">
         <v>56</v>
       </c>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="J125" t="str">
+        <f t="shared" si="3"/>
+        <v>00111000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>4220</v>
       </c>
       <c r="B126" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107C</v>
       </c>
       <c r="C126">
@@ -4209,13 +4705,17 @@
       <c r="I126">
         <v>50</v>
       </c>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="J126" t="str">
+        <f t="shared" si="3"/>
+        <v>00110010</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>4221</v>
       </c>
       <c r="B127" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107D</v>
       </c>
       <c r="C127">
@@ -4239,13 +4739,17 @@
       <c r="I127">
         <v>44</v>
       </c>
-    </row>
-    <row r="128" spans="1:9">
+      <c r="J127" t="str">
+        <f t="shared" si="3"/>
+        <v>00101100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>4222</v>
       </c>
       <c r="B128" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107E</v>
       </c>
       <c r="C128">
@@ -4269,13 +4773,17 @@
       <c r="I128">
         <v>38</v>
       </c>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="J128" t="str">
+        <f t="shared" si="3"/>
+        <v>00100110</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>4223</v>
       </c>
       <c r="B129" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107F</v>
       </c>
       <c r="C129">
@@ -4298,6 +4806,10 @@
       </c>
       <c r="I129">
         <v>32</v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" si="3"/>
+        <v>00100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>